<commit_message>
[Demo Project][Add Employee][Version 1][Write in Excel Sheet In progress, Need bug fixing]
</commit_message>
<xml_diff>
--- a/resources/testdata/ExcelFiles/TestDataWrite.xlsx
+++ b/resources/testdata/ExcelFiles/TestDataWrite.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DataDrivenSession\qa-repo\resources\testdata\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DemoProjectSeleniumJava\DemoProjectSeleniumJava\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD45A36-53E9-49F7-8A3C-B50B582ED037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6408" yWindow="1476" windowWidth="21600" windowHeight="11388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,18 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>করোনা সংক্রমণ বাড়াচ্ছে</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>0312</t>
+  </si>
+  <si>
+    <t>A8DCo 4Ys</t>
+  </si>
+  <si>
+    <t>010Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -355,23 +366,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Demo Project][Add Employee][Version 1][Add Employee Done, Write Excel bug fix needed]
</commit_message>
<xml_diff>
--- a/resources/testdata/ExcelFiles/TestDataWrite.xlsx
+++ b/resources/testdata/ExcelFiles/TestDataWrite.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DemoProjectSeleniumJava\DemoProjectSeleniumJava\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,31 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>0312</t>
+    <t>Employee ID</t>
   </si>
   <si>
-    <t>A8DCo 4Ys</t>
-  </si>
-  <si>
-    <t>010Z</t>
+    <t>First and Middle Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -58,18 +48,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,9 +68,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,38 +350,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="C4" t="s">
-        <v>5</v>
+      <c r="C1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Demo Project][Add Employee][Version 1][Add Employee Done, Write on Excel Done]
</commit_message>
<xml_diff>
--- a/resources/testdata/ExcelFiles/TestDataWrite.xlsx
+++ b/resources/testdata/ExcelFiles/TestDataWrite.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DemoProjectSeleniumJava\DemoProjectSeleniumJava\resources\testdata\ExcelFiles\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Last Name</t>
   </si>
@@ -33,12 +33,49 @@
   </si>
   <si>
     <t>First and Middle Name</t>
+  </si>
+  <si>
+    <t>4187</t>
+  </si>
+  <si>
+    <t>AgR6vFirstName 71Fm2MiddleName</t>
+  </si>
+  <si>
+    <t>AbZIhLastName</t>
+  </si>
+  <si>
+    <t>5318</t>
+  </si>
+  <si>
+    <t>QdquzFirstName wpmoAMiddleName</t>
+  </si>
+  <si>
+    <t>3fDcELastName</t>
+  </si>
+  <si>
+    <t>5012</t>
+  </si>
+  <si>
+    <t>ZuHNAFirstName qMOFcMiddleName</t>
+  </si>
+  <si>
+    <t>lgZgiLastName</t>
+  </si>
+  <si>
+    <t>8784</t>
+  </si>
+  <si>
+    <t>nnV3lFirstName AZz7dMiddleName</t>
+  </si>
+  <si>
+    <t>JJITYLastName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -358,20 +395,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>